<commit_message>
Lagt till 106 och 108 till distans skog och vatten. Tagit bort trivialnamnen från distansfilen som går upp på github. Lagt till 106 och 108 till lämmelsannolikhetsfilerna. Gjort en ny andel lämmelsannolikhet där jag delat upp efter tredjedelar. Den översta tredjedelen är bra. Mitten medelbra. Dålig lägst.
</commit_message>
<xml_diff>
--- a/Rawdata/andel_lämmelhabitattyper_per_lya.xlsx
+++ b/Rawdata/andel_lämmelhabitattyper_per_lya.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,10 +409,10 @@
         <v>361</v>
       </c>
       <c r="C2">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="D2">
-        <v>2435</v>
+        <v>2449</v>
       </c>
       <c r="E2">
         <v>3322</v>
@@ -421,10 +421,10 @@
         <v>0.1086694762191451</v>
       </c>
       <c r="G2">
-        <v>0.1583383503913305</v>
+        <v>0.1541240216736905</v>
       </c>
       <c r="H2">
-        <v>0.7329921733895244</v>
+        <v>0.7372065021071643</v>
       </c>
     </row>
     <row r="3">
@@ -437,10 +437,10 @@
         <v>1518</v>
       </c>
       <c r="C3">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="D3">
-        <v>1302</v>
+        <v>1309</v>
       </c>
       <c r="E3">
         <v>3330</v>
@@ -449,10 +449,10 @@
         <v>0.4558558558558559</v>
       </c>
       <c r="G3">
-        <v>0.1531531531531531</v>
+        <v>0.151051051051051</v>
       </c>
       <c r="H3">
-        <v>0.390990990990991</v>
+        <v>0.3930930930930931</v>
       </c>
     </row>
     <row r="4">
@@ -465,10 +465,10 @@
         <v>1883</v>
       </c>
       <c r="C4">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="D4">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="E4">
         <v>3325</v>
@@ -477,10 +477,10 @@
         <v>0.5663157894736842</v>
       </c>
       <c r="G4">
-        <v>0.2222556390977444</v>
+        <v>0.2207518796992481</v>
       </c>
       <c r="H4">
-        <v>0.2114285714285714</v>
+        <v>0.2129323308270677</v>
       </c>
     </row>
     <row r="5">
@@ -493,10 +493,10 @@
         <v>1316</v>
       </c>
       <c r="C5">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="D5">
-        <v>1445</v>
+        <v>1451</v>
       </c>
       <c r="E5">
         <v>3327</v>
@@ -505,10 +505,10 @@
         <v>0.395551547941088</v>
       </c>
       <c r="G5">
-        <v>0.1701232341448753</v>
+        <v>0.1683198076345055</v>
       </c>
       <c r="H5">
-        <v>0.4343252179140367</v>
+        <v>0.4361286444244064</v>
       </c>
     </row>
     <row r="6">
@@ -521,10 +521,10 @@
         <v>984</v>
       </c>
       <c r="C6">
-        <v>1036</v>
+        <v>1017</v>
       </c>
       <c r="D6">
-        <v>1304</v>
+        <v>1323</v>
       </c>
       <c r="E6">
         <v>3324</v>
@@ -533,10 +533,10 @@
         <v>0.296028880866426</v>
       </c>
       <c r="G6">
-        <v>0.3116726835138388</v>
+        <v>0.305956678700361</v>
       </c>
       <c r="H6">
-        <v>0.3922984356197353</v>
+        <v>0.398014440433213</v>
       </c>
     </row>
     <row r="7">
@@ -549,10 +549,10 @@
         <v>529</v>
       </c>
       <c r="C7">
-        <v>934</v>
+        <v>912</v>
       </c>
       <c r="D7">
-        <v>1860</v>
+        <v>1882</v>
       </c>
       <c r="E7">
         <v>3323</v>
@@ -561,10 +561,10 @@
         <v>0.1591934998495335</v>
       </c>
       <c r="G7">
-        <v>0.2810713210953957</v>
+        <v>0.2744507974721637</v>
       </c>
       <c r="H7">
-        <v>0.5597351790550708</v>
+        <v>0.5663557026783027</v>
       </c>
     </row>
     <row r="8">
@@ -577,10 +577,10 @@
         <v>1116</v>
       </c>
       <c r="C8">
-        <v>677</v>
+        <v>659</v>
       </c>
       <c r="D8">
-        <v>1107</v>
+        <v>1125</v>
       </c>
       <c r="E8">
         <v>2900</v>
@@ -589,10 +589,10 @@
         <v>0.3848275862068966</v>
       </c>
       <c r="G8">
-        <v>0.233448275862069</v>
+        <v>0.2272413793103448</v>
       </c>
       <c r="H8">
-        <v>0.3817241379310345</v>
+        <v>0.3879310344827586</v>
       </c>
     </row>
     <row r="9">
@@ -605,10 +605,10 @@
         <v>516</v>
       </c>
       <c r="C9">
-        <v>1347</v>
+        <v>1325</v>
       </c>
       <c r="D9">
-        <v>1462</v>
+        <v>1484</v>
       </c>
       <c r="E9">
         <v>3325</v>
@@ -617,10 +617,10 @@
         <v>0.155187969924812</v>
       </c>
       <c r="G9">
-        <v>0.4051127819548872</v>
+        <v>0.3984962406015037</v>
       </c>
       <c r="H9">
-        <v>0.4396992481203008</v>
+        <v>0.4463157894736842</v>
       </c>
     </row>
     <row r="10">
@@ -633,10 +633,10 @@
         <v>561</v>
       </c>
       <c r="C10">
-        <v>1124</v>
+        <v>1096</v>
       </c>
       <c r="D10">
-        <v>1637</v>
+        <v>1665</v>
       </c>
       <c r="E10">
         <v>3322</v>
@@ -645,10 +645,10 @@
         <v>0.1688741721854305</v>
       </c>
       <c r="G10">
-        <v>0.3383503913305238</v>
+        <v>0.3299217338952438</v>
       </c>
       <c r="H10">
-        <v>0.4927754364840458</v>
+        <v>0.5012040939193257</v>
       </c>
     </row>
     <row r="11">
@@ -661,10 +661,10 @@
         <v>964</v>
       </c>
       <c r="C11">
-        <v>1275</v>
+        <v>1252</v>
       </c>
       <c r="D11">
-        <v>1088</v>
+        <v>1111</v>
       </c>
       <c r="E11">
         <v>3327</v>
@@ -673,10 +673,10 @@
         <v>0.2897505259993989</v>
       </c>
       <c r="G11">
-        <v>0.3832281334535618</v>
+        <v>0.3763149984971446</v>
       </c>
       <c r="H11">
-        <v>0.3270213405470394</v>
+        <v>0.3339344755034566</v>
       </c>
     </row>
     <row r="12">
@@ -689,10 +689,10 @@
         <v>530</v>
       </c>
       <c r="C12">
-        <v>914</v>
+        <v>900</v>
       </c>
       <c r="D12">
-        <v>1874</v>
+        <v>1888</v>
       </c>
       <c r="E12">
         <v>3318</v>
@@ -701,10 +701,10 @@
         <v>0.1597347799879446</v>
       </c>
       <c r="G12">
-        <v>0.2754671488848704</v>
+        <v>0.27124773960217</v>
       </c>
       <c r="H12">
-        <v>0.5647980711271851</v>
+        <v>0.5690174804098854</v>
       </c>
     </row>
     <row r="13">
@@ -717,10 +717,10 @@
         <v>985</v>
       </c>
       <c r="C13">
-        <v>1104</v>
+        <v>1085</v>
       </c>
       <c r="D13">
-        <v>1236</v>
+        <v>1255</v>
       </c>
       <c r="E13">
         <v>3325</v>
@@ -729,10 +729,10 @@
         <v>0.2962406015037594</v>
       </c>
       <c r="G13">
-        <v>0.3320300751879699</v>
+        <v>0.3263157894736842</v>
       </c>
       <c r="H13">
-        <v>0.3717293233082707</v>
+        <v>0.3774436090225564</v>
       </c>
     </row>
     <row r="14">
@@ -745,10 +745,10 @@
         <v>756</v>
       </c>
       <c r="C14">
-        <v>780</v>
+        <v>756</v>
       </c>
       <c r="D14">
-        <v>1790</v>
+        <v>1814</v>
       </c>
       <c r="E14">
         <v>3326</v>
@@ -757,10 +757,10 @@
         <v>0.227300060132291</v>
       </c>
       <c r="G14">
-        <v>0.2345159350571257</v>
+        <v>0.227300060132291</v>
       </c>
       <c r="H14">
-        <v>0.5381840048105833</v>
+        <v>0.5453998797354179</v>
       </c>
     </row>
     <row r="15">
@@ -773,10 +773,10 @@
         <v>957</v>
       </c>
       <c r="C15">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="D15">
-        <v>1883</v>
+        <v>1895</v>
       </c>
       <c r="E15">
         <v>3329</v>
@@ -785,10 +785,10 @@
         <v>0.2874737158305797</v>
       </c>
       <c r="G15">
-        <v>0.1468909582457194</v>
+        <v>0.1432862721537999</v>
       </c>
       <c r="H15">
-        <v>0.5656353259237008</v>
+        <v>0.5692400120156204</v>
       </c>
     </row>
     <row r="16">
@@ -801,10 +801,10 @@
         <v>628</v>
       </c>
       <c r="C16">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="D16">
-        <v>2364</v>
+        <v>2377</v>
       </c>
       <c r="E16">
         <v>3326</v>
@@ -813,10 +813,10 @@
         <v>0.1888153938665063</v>
       </c>
       <c r="G16">
-        <v>0.100420926037282</v>
+        <v>0.09651232711966326</v>
       </c>
       <c r="H16">
-        <v>0.7107636800962117</v>
+        <v>0.7146722790138305</v>
       </c>
     </row>
     <row r="17">
@@ -829,10 +829,10 @@
         <v>963</v>
       </c>
       <c r="C17">
-        <v>356</v>
+        <v>339</v>
       </c>
       <c r="D17">
-        <v>1998</v>
+        <v>2015</v>
       </c>
       <c r="E17">
         <v>3317</v>
@@ -841,10 +841,10 @@
         <v>0.2903225806451613</v>
       </c>
       <c r="G17">
-        <v>0.1073258968947844</v>
+        <v>0.10220078384082</v>
       </c>
       <c r="H17">
-        <v>0.6023515224600543</v>
+        <v>0.6074766355140186</v>
       </c>
     </row>
     <row r="18">
@@ -857,10 +857,10 @@
         <v>904</v>
       </c>
       <c r="C18">
-        <v>1228</v>
+        <v>1196</v>
       </c>
       <c r="D18">
-        <v>1195</v>
+        <v>1227</v>
       </c>
       <c r="E18">
         <v>3327</v>
@@ -869,10 +869,10 @@
         <v>0.2717162608957018</v>
       </c>
       <c r="G18">
-        <v>0.3691012924556658</v>
+        <v>0.359483017733694</v>
       </c>
       <c r="H18">
-        <v>0.3591824466486324</v>
+        <v>0.3688007213706042</v>
       </c>
     </row>
     <row r="19">
@@ -885,10 +885,10 @@
         <v>51</v>
       </c>
       <c r="C19">
-        <v>587</v>
+        <v>565</v>
       </c>
       <c r="D19">
-        <v>2678</v>
+        <v>2700</v>
       </c>
       <c r="E19">
         <v>3316</v>
@@ -897,10 +897,10 @@
         <v>0.01537997587454765</v>
       </c>
       <c r="G19">
-        <v>0.1770205066344994</v>
+        <v>0.1703860072376357</v>
       </c>
       <c r="H19">
-        <v>0.8075995174909529</v>
+        <v>0.8142340168878166</v>
       </c>
     </row>
     <row r="20">
@@ -913,10 +913,10 @@
         <v>176</v>
       </c>
       <c r="C20">
-        <v>493</v>
+        <v>471</v>
       </c>
       <c r="D20">
-        <v>2656</v>
+        <v>2678</v>
       </c>
       <c r="E20">
         <v>3325</v>
@@ -925,10 +925,10 @@
         <v>0.05293233082706767</v>
       </c>
       <c r="G20">
-        <v>0.1482706766917293</v>
+        <v>0.1416541353383459</v>
       </c>
       <c r="H20">
-        <v>0.7987969924812031</v>
+        <v>0.8054135338345865</v>
       </c>
     </row>
     <row r="21">
@@ -941,10 +941,10 @@
         <v>316</v>
       </c>
       <c r="C21">
-        <v>962</v>
+        <v>930</v>
       </c>
       <c r="D21">
-        <v>2043</v>
+        <v>2075</v>
       </c>
       <c r="E21">
         <v>3321</v>
@@ -953,10 +953,10 @@
         <v>0.09515206263173742</v>
       </c>
       <c r="G21">
-        <v>0.2896717856067449</v>
+        <v>0.2800361336946703</v>
       </c>
       <c r="H21">
-        <v>0.6151761517615176</v>
+        <v>0.6248118036735922</v>
       </c>
     </row>
     <row r="22">
@@ -969,10 +969,10 @@
         <v>510</v>
       </c>
       <c r="C22">
-        <v>1160</v>
+        <v>1138</v>
       </c>
       <c r="D22">
-        <v>1648</v>
+        <v>1670</v>
       </c>
       <c r="E22">
         <v>3318</v>
@@ -981,10 +981,10 @@
         <v>0.1537070524412296</v>
       </c>
       <c r="G22">
-        <v>0.3496081977094636</v>
+        <v>0.3429776974080772</v>
       </c>
       <c r="H22">
-        <v>0.4966847498493068</v>
+        <v>0.5033152501506932</v>
       </c>
     </row>
     <row r="23">
@@ -997,10 +997,10 @@
         <v>801</v>
       </c>
       <c r="C23">
-        <v>1017</v>
+        <v>1002</v>
       </c>
       <c r="D23">
-        <v>1504</v>
+        <v>1519</v>
       </c>
       <c r="E23">
         <v>3322</v>
@@ -1009,10 +1009,10 @@
         <v>0.2411198073449729</v>
       </c>
       <c r="G23">
-        <v>0.3061408789885611</v>
+        <v>0.3016255267910897</v>
       </c>
       <c r="H23">
-        <v>0.452739313666466</v>
+        <v>0.4572546658639374</v>
       </c>
     </row>
     <row r="24">
@@ -1025,10 +1025,10 @@
         <v>193</v>
       </c>
       <c r="C24">
-        <v>600</v>
+        <v>587</v>
       </c>
       <c r="D24">
-        <v>2538</v>
+        <v>2551</v>
       </c>
       <c r="E24">
         <v>3331</v>
@@ -1037,10 +1037,10 @@
         <v>0.05794055839087361</v>
       </c>
       <c r="G24">
-        <v>0.1801260882617833</v>
+        <v>0.1762233563494446</v>
       </c>
       <c r="H24">
-        <v>0.7619333533473431</v>
+        <v>0.7658360852596818</v>
       </c>
     </row>
     <row r="25">
@@ -1053,10 +1053,10 @@
         <v>863</v>
       </c>
       <c r="C25">
-        <v>1136</v>
+        <v>1124</v>
       </c>
       <c r="D25">
-        <v>1333</v>
+        <v>1345</v>
       </c>
       <c r="E25">
         <v>3332</v>
@@ -1065,10 +1065,10 @@
         <v>0.2590036014405762</v>
       </c>
       <c r="G25">
-        <v>0.34093637454982</v>
+        <v>0.3373349339735894</v>
       </c>
       <c r="H25">
-        <v>0.4000600240096038</v>
+        <v>0.4036614645858344</v>
       </c>
     </row>
     <row r="26">
@@ -1081,10 +1081,10 @@
         <v>405</v>
       </c>
       <c r="C26">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="D26">
-        <v>2248</v>
+        <v>2261</v>
       </c>
       <c r="E26">
         <v>3325</v>
@@ -1093,10 +1093,10 @@
         <v>0.1218045112781955</v>
       </c>
       <c r="G26">
-        <v>0.2021052631578947</v>
+        <v>0.1981954887218045</v>
       </c>
       <c r="H26">
-        <v>0.6760902255639097</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="27">
@@ -1137,10 +1137,10 @@
         <v>259</v>
       </c>
       <c r="C28">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D28">
-        <v>2863</v>
+        <v>2872</v>
       </c>
       <c r="E28">
         <v>3319</v>
@@ -1149,10 +1149,10 @@
         <v>0.0780355528773727</v>
       </c>
       <c r="G28">
-        <v>0.05935522747815607</v>
+        <v>0.05664356733956011</v>
       </c>
       <c r="H28">
-        <v>0.8626092196444712</v>
+        <v>0.8653208797830672</v>
       </c>
     </row>
     <row r="29">
@@ -1165,10 +1165,10 @@
         <v>1944</v>
       </c>
       <c r="C29">
-        <v>846</v>
+        <v>831</v>
       </c>
       <c r="D29">
-        <v>536</v>
+        <v>551</v>
       </c>
       <c r="E29">
         <v>3326</v>
@@ -1177,10 +1177,10 @@
         <v>0.5844858689116055</v>
       </c>
       <c r="G29">
-        <v>0.2543595911004209</v>
+        <v>0.2498496692723993</v>
       </c>
       <c r="H29">
-        <v>0.1611545399879735</v>
+        <v>0.1656644618159952</v>
       </c>
     </row>
     <row r="30">
@@ -1193,10 +1193,10 @@
         <v>500</v>
       </c>
       <c r="C30">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D30">
-        <v>2467</v>
+        <v>2475</v>
       </c>
       <c r="E30">
         <v>3325</v>
@@ -1205,10 +1205,10 @@
         <v>0.1503759398496241</v>
       </c>
       <c r="G30">
-        <v>0.1076691729323308</v>
+        <v>0.1052631578947368</v>
       </c>
       <c r="H30">
-        <v>0.7419548872180451</v>
+        <v>0.7443609022556391</v>
       </c>
     </row>
     <row r="31">
@@ -1221,10 +1221,10 @@
         <v>1634</v>
       </c>
       <c r="C31">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="D31">
-        <v>1358</v>
+        <v>1364</v>
       </c>
       <c r="E31">
         <v>3318</v>
@@ -1233,10 +1233,10 @@
         <v>0.4924653405666064</v>
       </c>
       <c r="G31">
-        <v>0.09825195901145269</v>
+        <v>0.09644364074743822</v>
       </c>
       <c r="H31">
-        <v>0.4092827004219409</v>
+        <v>0.4110910186859554</v>
       </c>
     </row>
     <row r="32">
@@ -1249,10 +1249,10 @@
         <v>270</v>
       </c>
       <c r="C32">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D32">
-        <v>2804</v>
+        <v>2810</v>
       </c>
       <c r="E32">
         <v>3330</v>
@@ -1261,10 +1261,10 @@
         <v>0.08108108108108109</v>
       </c>
       <c r="G32">
-        <v>0.07687687687687687</v>
+        <v>0.07507507507507508</v>
       </c>
       <c r="H32">
-        <v>0.842042042042042</v>
+        <v>0.8438438438438438</v>
       </c>
     </row>
     <row r="33">
@@ -1277,10 +1277,10 @@
         <v>60</v>
       </c>
       <c r="C33">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D33">
-        <v>3082</v>
+        <v>3088</v>
       </c>
       <c r="E33">
         <v>3329</v>
@@ -1289,10 +1289,10 @@
         <v>0.01802343045959748</v>
       </c>
       <c r="G33">
-        <v>0.05617302493241214</v>
+        <v>0.05437068188645239</v>
       </c>
       <c r="H33">
-        <v>0.9258035446079904</v>
+        <v>0.9276058876539501</v>
       </c>
     </row>
     <row r="34">
@@ -1305,10 +1305,10 @@
         <v>46</v>
       </c>
       <c r="C34">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D34">
-        <v>3125</v>
+        <v>3131</v>
       </c>
       <c r="E34">
         <v>3318</v>
@@ -1317,10 +1317,10 @@
         <v>0.01386377335744424</v>
       </c>
       <c r="G34">
-        <v>0.04430379746835443</v>
+        <v>0.04249547920433996</v>
       </c>
       <c r="H34">
-        <v>0.9418324291742013</v>
+        <v>0.9436407474382158</v>
       </c>
     </row>
     <row r="35">
@@ -1333,10 +1333,10 @@
         <v>130</v>
       </c>
       <c r="C35">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="D35">
-        <v>2788</v>
+        <v>2804</v>
       </c>
       <c r="E35">
         <v>3325</v>
@@ -1345,10 +1345,10 @@
         <v>0.03909774436090226</v>
       </c>
       <c r="G35">
-        <v>0.122406015037594</v>
+        <v>0.117593984962406</v>
       </c>
       <c r="H35">
-        <v>0.8384962406015037</v>
+        <v>0.8433082706766918</v>
       </c>
     </row>
     <row r="36">
@@ -1361,10 +1361,10 @@
         <v>441</v>
       </c>
       <c r="C36">
-        <v>729</v>
+        <v>714</v>
       </c>
       <c r="D36">
-        <v>2154</v>
+        <v>2169</v>
       </c>
       <c r="E36">
         <v>3324</v>
@@ -1373,10 +1373,10 @@
         <v>0.1326714801444043</v>
       </c>
       <c r="G36">
-        <v>0.2193140794223827</v>
+        <v>0.2148014440433213</v>
       </c>
       <c r="H36">
-        <v>0.648014440433213</v>
+        <v>0.6525270758122743</v>
       </c>
     </row>
     <row r="37">
@@ -1389,10 +1389,10 @@
         <v>699</v>
       </c>
       <c r="C37">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="D37">
-        <v>2328</v>
+        <v>2337</v>
       </c>
       <c r="E37">
         <v>3318</v>
@@ -1401,10 +1401,10 @@
         <v>0.2106690777576853</v>
       </c>
       <c r="G37">
-        <v>0.08770343580470162</v>
+        <v>0.08499095840867993</v>
       </c>
       <c r="H37">
-        <v>0.701627486437613</v>
+        <v>0.7043399638336347</v>
       </c>
     </row>
     <row r="38">
@@ -1417,10 +1417,10 @@
         <v>104</v>
       </c>
       <c r="C38">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D38">
-        <v>3033</v>
+        <v>3035</v>
       </c>
       <c r="E38">
         <v>3319</v>
@@ -1429,10 +1429,10 @@
         <v>0.03133473937933112</v>
       </c>
       <c r="G38">
-        <v>0.05483579391382946</v>
+        <v>0.05423320277191925</v>
       </c>
       <c r="H38">
-        <v>0.9138294667068394</v>
+        <v>0.9144320578487496</v>
       </c>
     </row>
     <row r="39">
@@ -1445,10 +1445,10 @@
         <v>474</v>
       </c>
       <c r="C39">
-        <v>913</v>
+        <v>898</v>
       </c>
       <c r="D39">
-        <v>1938</v>
+        <v>1953</v>
       </c>
       <c r="E39">
         <v>3325</v>
@@ -1457,10 +1457,10 @@
         <v>0.1425563909774436</v>
       </c>
       <c r="G39">
-        <v>0.2745864661654135</v>
+        <v>0.2700751879699248</v>
       </c>
       <c r="H39">
-        <v>0.5828571428571429</v>
+        <v>0.5873684210526315</v>
       </c>
     </row>
     <row r="40">
@@ -1473,10 +1473,10 @@
         <v>1096</v>
       </c>
       <c r="C40">
-        <v>1026</v>
+        <v>1002</v>
       </c>
       <c r="D40">
-        <v>1205</v>
+        <v>1229</v>
       </c>
       <c r="E40">
         <v>3327</v>
@@ -1485,10 +1485,10 @@
         <v>0.3294259092275323</v>
       </c>
       <c r="G40">
-        <v>0.3083859332732191</v>
+        <v>0.3011722272317403</v>
       </c>
       <c r="H40">
-        <v>0.3621881574992486</v>
+        <v>0.3694018635407274</v>
       </c>
     </row>
     <row r="41">
@@ -1501,10 +1501,10 @@
         <v>229</v>
       </c>
       <c r="C41">
-        <v>358</v>
+        <v>329</v>
       </c>
       <c r="D41">
-        <v>2739</v>
+        <v>2768</v>
       </c>
       <c r="E41">
         <v>3326</v>
@@ -1513,10 +1513,10 @@
         <v>0.06885147324113049</v>
       </c>
       <c r="G41">
-        <v>0.1076368009621167</v>
+        <v>0.09891761876127481</v>
       </c>
       <c r="H41">
-        <v>0.8235117257967528</v>
+        <v>0.8322309079975947</v>
       </c>
     </row>
     <row r="42">
@@ -1529,10 +1529,10 @@
         <v>420</v>
       </c>
       <c r="C42">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D42">
-        <v>2721</v>
+        <v>2724</v>
       </c>
       <c r="E42">
         <v>3327</v>
@@ -1541,10 +1541,10 @@
         <v>0.1262398557258792</v>
       </c>
       <c r="G42">
-        <v>0.05590622182146077</v>
+        <v>0.05500450856627592</v>
       </c>
       <c r="H42">
-        <v>0.8178539224526601</v>
+        <v>0.8187556357078449</v>
       </c>
     </row>
     <row r="43">
@@ -1557,10 +1557,10 @@
         <v>428</v>
       </c>
       <c r="C43">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D43">
-        <v>2408</v>
+        <v>2411</v>
       </c>
       <c r="E43">
         <v>3321</v>
@@ -1569,10 +1569,10 @@
         <v>0.1288768443239988</v>
       </c>
       <c r="G43">
-        <v>0.1460403492923818</v>
+        <v>0.1451370069256248</v>
       </c>
       <c r="H43">
-        <v>0.7250828063836194</v>
+        <v>0.7259861487503764</v>
       </c>
     </row>
     <row r="44">
@@ -1585,10 +1585,10 @@
         <v>555</v>
       </c>
       <c r="C44">
-        <v>926</v>
+        <v>910</v>
       </c>
       <c r="D44">
-        <v>1842</v>
+        <v>1858</v>
       </c>
       <c r="E44">
         <v>3323</v>
@@ -1597,10 +1597,10 @@
         <v>0.1670177550406259</v>
       </c>
       <c r="G44">
-        <v>0.278663857959675</v>
+        <v>0.2738489316882335</v>
       </c>
       <c r="H44">
-        <v>0.554318386999699</v>
+        <v>0.5591333132711406</v>
       </c>
     </row>
     <row r="45">
@@ -1613,10 +1613,10 @@
         <v>1671</v>
       </c>
       <c r="C45">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="D45">
-        <v>1066</v>
+        <v>1073</v>
       </c>
       <c r="E45">
         <v>3318</v>
@@ -1625,10 +1625,10 @@
         <v>0.5036166365280289</v>
       </c>
       <c r="G45">
-        <v>0.1751054852320675</v>
+        <v>0.1729957805907173</v>
       </c>
       <c r="H45">
-        <v>0.3212778782399036</v>
+        <v>0.3233875828812537</v>
       </c>
     </row>
     <row r="46">
@@ -1641,10 +1641,10 @@
         <v>2264</v>
       </c>
       <c r="C46">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="D46">
-        <v>558</v>
+        <v>570</v>
       </c>
       <c r="E46">
         <v>3321</v>
@@ -1653,10 +1653,10 @@
         <v>0.6817223727792834</v>
       </c>
       <c r="G46">
-        <v>0.1502559470039145</v>
+        <v>0.1466425775368865</v>
       </c>
       <c r="H46">
-        <v>0.1680216802168022</v>
+        <v>0.1716350496838302</v>
       </c>
     </row>
     <row r="47">
@@ -1669,10 +1669,10 @@
         <v>1613</v>
       </c>
       <c r="C47">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="D47">
-        <v>1224</v>
+        <v>1238</v>
       </c>
       <c r="E47">
         <v>3327</v>
@@ -1681,10 +1681,10 @@
         <v>0.4848211602043883</v>
       </c>
       <c r="G47">
-        <v>0.1472798316801924</v>
+        <v>0.1430718364893297</v>
       </c>
       <c r="H47">
-        <v>0.3678990081154193</v>
+        <v>0.3721070033062819</v>
       </c>
     </row>
     <row r="48">
@@ -1697,10 +1697,10 @@
         <v>1494</v>
       </c>
       <c r="C48">
-        <v>1092</v>
+        <v>1079</v>
       </c>
       <c r="D48">
-        <v>742</v>
+        <v>755</v>
       </c>
       <c r="E48">
         <v>3328</v>
@@ -1709,10 +1709,10 @@
         <v>0.4489182692307692</v>
       </c>
       <c r="G48">
-        <v>0.328125</v>
+        <v>0.32421875</v>
       </c>
       <c r="H48">
-        <v>0.2229567307692308</v>
+        <v>0.2268629807692308</v>
       </c>
     </row>
     <row r="49">
@@ -1725,10 +1725,10 @@
         <v>250</v>
       </c>
       <c r="C49">
-        <v>731</v>
+        <v>721</v>
       </c>
       <c r="D49">
-        <v>2346</v>
+        <v>2356</v>
       </c>
       <c r="E49">
         <v>3327</v>
@@ -1737,10 +1737,10 @@
         <v>0.07514277126540427</v>
       </c>
       <c r="G49">
-        <v>0.2197174631800421</v>
+        <v>0.2167117523294259</v>
       </c>
       <c r="H49">
-        <v>0.7051397655545536</v>
+        <v>0.7081454764051698</v>
       </c>
     </row>
     <row r="50">
@@ -1753,10 +1753,10 @@
         <v>848</v>
       </c>
       <c r="C50">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D50">
-        <v>2270</v>
+        <v>2272</v>
       </c>
       <c r="E50">
         <v>3325</v>
@@ -1765,10 +1765,10 @@
         <v>0.2550375939849624</v>
       </c>
       <c r="G50">
-        <v>0.06225563909774436</v>
+        <v>0.06165413533834586</v>
       </c>
       <c r="H50">
-        <v>0.6827067669172933</v>
+        <v>0.6833082706766918</v>
       </c>
     </row>
     <row r="51">
@@ -1781,10 +1781,10 @@
         <v>110</v>
       </c>
       <c r="C51">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D51">
-        <v>3089</v>
+        <v>3098</v>
       </c>
       <c r="E51">
         <v>3326</v>
@@ -1793,10 +1793,10 @@
         <v>0.03307276007215875</v>
       </c>
       <c r="G51">
-        <v>0.03818400481058328</v>
+        <v>0.0354780517137703</v>
       </c>
       <c r="H51">
-        <v>0.928743235117258</v>
+        <v>0.931449188214071</v>
       </c>
     </row>
     <row r="52">
@@ -1809,10 +1809,10 @@
         <v>41</v>
       </c>
       <c r="C52">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="D52">
-        <v>2990</v>
+        <v>3005</v>
       </c>
       <c r="E52">
         <v>3319</v>
@@ -1821,10 +1821,10 @@
         <v>0.01235311840915938</v>
       </c>
       <c r="G52">
-        <v>0.08677312443507081</v>
+        <v>0.0822536908707442</v>
       </c>
       <c r="H52">
-        <v>0.9008737571557698</v>
+        <v>0.9053931907200964</v>
       </c>
     </row>
     <row r="53">
@@ -1837,10 +1837,10 @@
         <v>34</v>
       </c>
       <c r="C53">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D53">
-        <v>3173</v>
+        <v>3175</v>
       </c>
       <c r="E53">
         <v>3325</v>
@@ -1849,10 +1849,10 @@
         <v>0.01022556390977444</v>
       </c>
       <c r="G53">
-        <v>0.03548872180451128</v>
+        <v>0.03488721804511278</v>
       </c>
       <c r="H53">
-        <v>0.9542857142857143</v>
+        <v>0.9548872180451128</v>
       </c>
     </row>
     <row r="54">
@@ -1865,10 +1865,10 @@
         <v>1213</v>
       </c>
       <c r="C54">
-        <v>927</v>
+        <v>915</v>
       </c>
       <c r="D54">
-        <v>1186</v>
+        <v>1198</v>
       </c>
       <c r="E54">
         <v>3326</v>
@@ -1877,10 +1877,10 @@
         <v>0.3647023451593506</v>
       </c>
       <c r="G54">
-        <v>0.2787131689717378</v>
+        <v>0.2751052315093205</v>
       </c>
       <c r="H54">
-        <v>0.3565844858689116</v>
+        <v>0.3601924233313289</v>
       </c>
     </row>
     <row r="55">
@@ -1893,10 +1893,10 @@
         <v>202</v>
       </c>
       <c r="C55">
-        <v>915</v>
+        <v>893</v>
       </c>
       <c r="D55">
-        <v>2214</v>
+        <v>2236</v>
       </c>
       <c r="E55">
         <v>3331</v>
@@ -1905,10 +1905,10 @@
         <v>0.06064244971480036</v>
       </c>
       <c r="G55">
-        <v>0.2746922845992195</v>
+        <v>0.2680876613629541</v>
       </c>
       <c r="H55">
-        <v>0.6646652656859802</v>
+        <v>0.6712698889222456</v>
       </c>
     </row>
     <row r="56">
@@ -1921,10 +1921,10 @@
         <v>69</v>
       </c>
       <c r="C56">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D56">
-        <v>3094</v>
+        <v>3098</v>
       </c>
       <c r="E56">
         <v>3315</v>
@@ -1933,10 +1933,10 @@
         <v>0.02081447963800905</v>
       </c>
       <c r="G56">
-        <v>0.04585218702865761</v>
+        <v>0.04464555052790347</v>
       </c>
       <c r="H56">
-        <v>0.9333333333333333</v>
+        <v>0.9345399698340875</v>
       </c>
     </row>
     <row r="57">
@@ -1949,10 +1949,10 @@
         <v>878</v>
       </c>
       <c r="C57">
-        <v>1327</v>
+        <v>1291</v>
       </c>
       <c r="D57">
-        <v>1112</v>
+        <v>1148</v>
       </c>
       <c r="E57">
         <v>3317</v>
@@ -1961,10 +1961,10 @@
         <v>0.2646970153753392</v>
       </c>
       <c r="G57">
-        <v>0.4000602954476937</v>
+        <v>0.3892071148628278</v>
       </c>
       <c r="H57">
-        <v>0.3352426891769671</v>
+        <v>0.346095869761833</v>
       </c>
     </row>
     <row r="58">
@@ -1977,10 +1977,10 @@
         <v>145</v>
       </c>
       <c r="C58">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D58">
-        <v>3119</v>
+        <v>3123</v>
       </c>
       <c r="E58">
         <v>3326</v>
@@ -1989,10 +1989,10 @@
         <v>0.04359591100420926</v>
       </c>
       <c r="G58">
-        <v>0.01864101022248948</v>
+        <v>0.0174383644016837</v>
       </c>
       <c r="H58">
-        <v>0.9377630787733012</v>
+        <v>0.938965724594107</v>
       </c>
     </row>
     <row r="59">
@@ -2005,10 +2005,10 @@
         <v>119</v>
       </c>
       <c r="C59">
-        <v>995</v>
+        <v>961</v>
       </c>
       <c r="D59">
-        <v>2204</v>
+        <v>2238</v>
       </c>
       <c r="E59">
         <v>3318</v>
@@ -2017,10 +2017,10 @@
         <v>0.03586497890295359</v>
       </c>
       <c r="G59">
-        <v>0.2998794454490657</v>
+        <v>0.2896323086196504</v>
       </c>
       <c r="H59">
-        <v>0.6642555756479807</v>
+        <v>0.674502712477396</v>
       </c>
     </row>
     <row r="60">
@@ -2033,10 +2033,10 @@
         <v>1586</v>
       </c>
       <c r="C60">
-        <v>709</v>
+        <v>703</v>
       </c>
       <c r="D60">
-        <v>1028</v>
+        <v>1034</v>
       </c>
       <c r="E60">
         <v>3323</v>
@@ -2045,10 +2045,10 @@
         <v>0.4772795666566356</v>
       </c>
       <c r="G60">
-        <v>0.2133614204032501</v>
+        <v>0.2115558230514595</v>
       </c>
       <c r="H60">
-        <v>0.3093590129401144</v>
+        <v>0.3111646102919049</v>
       </c>
     </row>
     <row r="61">
@@ -2061,10 +2061,10 @@
         <v>2</v>
       </c>
       <c r="C61">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D61">
-        <v>3265</v>
+        <v>3267</v>
       </c>
       <c r="E61">
         <v>3324</v>
@@ -2073,10 +2073,10 @@
         <v>0.0006016847172081829</v>
       </c>
       <c r="G61">
-        <v>0.01714801444043321</v>
+        <v>0.01654632972322503</v>
       </c>
       <c r="H61">
-        <v>0.9822503008423586</v>
+        <v>0.9828519855595668</v>
       </c>
     </row>
     <row r="62">
@@ -2089,10 +2089,10 @@
         <v>7</v>
       </c>
       <c r="C62">
-        <v>493</v>
+        <v>458</v>
       </c>
       <c r="D62">
-        <v>2419</v>
+        <v>2454</v>
       </c>
       <c r="E62">
         <v>2919</v>
@@ -2101,10 +2101,10 @@
         <v>0.002398081534772182</v>
       </c>
       <c r="G62">
-        <v>0.1688934566632408</v>
+        <v>0.1569030489893799</v>
       </c>
       <c r="H62">
-        <v>0.828708461801987</v>
+        <v>0.8406988694758479</v>
       </c>
     </row>
     <row r="63">
@@ -2117,10 +2117,10 @@
         <v>934</v>
       </c>
       <c r="C63">
-        <v>785</v>
+        <v>770</v>
       </c>
       <c r="D63">
-        <v>1603</v>
+        <v>1618</v>
       </c>
       <c r="E63">
         <v>3322</v>
@@ -2129,10 +2129,10 @@
         <v>0.2811559301625527</v>
       </c>
       <c r="G63">
-        <v>0.2363034316676701</v>
+        <v>0.2317880794701987</v>
       </c>
       <c r="H63">
-        <v>0.4825406381697773</v>
+        <v>0.4870559903672487</v>
       </c>
     </row>
     <row r="64">
@@ -2145,10 +2145,10 @@
         <v>7</v>
       </c>
       <c r="C64">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D64">
-        <v>3181</v>
+        <v>3188</v>
       </c>
       <c r="E64">
         <v>3325</v>
@@ -2157,10 +2157,10 @@
         <v>0.002105263157894737</v>
       </c>
       <c r="G64">
-        <v>0.04120300751879699</v>
+        <v>0.03909774436090226</v>
       </c>
       <c r="H64">
-        <v>0.9566917293233083</v>
+        <v>0.958796992481203</v>
       </c>
     </row>
     <row r="65">
@@ -2173,10 +2173,10 @@
         <v>371</v>
       </c>
       <c r="C65">
-        <v>783</v>
+        <v>770</v>
       </c>
       <c r="D65">
-        <v>2175</v>
+        <v>2188</v>
       </c>
       <c r="E65">
         <v>3329</v>
@@ -2185,10 +2185,10 @@
         <v>0.1114448783418444</v>
       </c>
       <c r="G65">
-        <v>0.2352057674977471</v>
+        <v>0.2313006908981676</v>
       </c>
       <c r="H65">
-        <v>0.6533493541604085</v>
+        <v>0.657254430759988</v>
       </c>
     </row>
     <row r="66">
@@ -2201,10 +2201,10 @@
         <v>555</v>
       </c>
       <c r="C66">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D66">
-        <v>2586</v>
+        <v>2588</v>
       </c>
       <c r="E66">
         <v>3326</v>
@@ -2213,10 +2213,10 @@
         <v>0.166867107636801</v>
       </c>
       <c r="G66">
-        <v>0.05562236921226699</v>
+        <v>0.0550210463018641</v>
       </c>
       <c r="H66">
-        <v>0.7775105231509321</v>
+        <v>0.778111846061335</v>
       </c>
     </row>
     <row r="67">
@@ -2229,10 +2229,10 @@
         <v>106</v>
       </c>
       <c r="C67">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="D67">
-        <v>2930</v>
+        <v>2939</v>
       </c>
       <c r="E67">
         <v>3324</v>
@@ -2241,10 +2241,10 @@
         <v>0.03188929001203369</v>
       </c>
       <c r="G67">
-        <v>0.08664259927797834</v>
+        <v>0.08393501805054152</v>
       </c>
       <c r="H67">
-        <v>0.881468110709988</v>
+        <v>0.8841756919374247</v>
       </c>
     </row>
     <row r="68">
@@ -2257,10 +2257,10 @@
         <v>504</v>
       </c>
       <c r="C68">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="D68">
-        <v>2316</v>
+        <v>2324</v>
       </c>
       <c r="E68">
         <v>3323</v>
@@ -2269,10 +2269,10 @@
         <v>0.1516701775504063</v>
       </c>
       <c r="G68">
-        <v>0.1513692446584412</v>
+        <v>0.1489617815227204</v>
       </c>
       <c r="H68">
-        <v>0.6969605777911526</v>
+        <v>0.6993680409268733</v>
       </c>
     </row>
     <row r="69">
@@ -2285,10 +2285,10 @@
         <v>131</v>
       </c>
       <c r="C69">
-        <v>922</v>
+        <v>886</v>
       </c>
       <c r="D69">
-        <v>2269</v>
+        <v>2305</v>
       </c>
       <c r="E69">
         <v>3322</v>
@@ -2297,10 +2297,10 @@
         <v>0.03943407585791692</v>
       </c>
       <c r="G69">
-        <v>0.2775436484045756</v>
+        <v>0.2667068031306442</v>
       </c>
       <c r="H69">
-        <v>0.6830222757375075</v>
+        <v>0.6938591210114389</v>
       </c>
     </row>
     <row r="70">
@@ -2313,10 +2313,10 @@
         <v>67</v>
       </c>
       <c r="C70">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D70">
-        <v>3123</v>
+        <v>3129</v>
       </c>
       <c r="E70">
         <v>3326</v>
@@ -2325,10 +2325,10 @@
         <v>0.02014431749849669</v>
       </c>
       <c r="G70">
-        <v>0.04088995790739627</v>
+        <v>0.03908598917618761</v>
       </c>
       <c r="H70">
-        <v>0.938965724594107</v>
+        <v>0.9407696933253157</v>
       </c>
     </row>
     <row r="71">
@@ -2341,10 +2341,10 @@
         <v>66</v>
       </c>
       <c r="C71">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="D71">
-        <v>2853</v>
+        <v>2861</v>
       </c>
       <c r="E71">
         <v>3328</v>
@@ -2353,10 +2353,10 @@
         <v>0.01983173076923077</v>
       </c>
       <c r="G71">
-        <v>0.1228966346153846</v>
+        <v>0.1204927884615385</v>
       </c>
       <c r="H71">
-        <v>0.8572716346153846</v>
+        <v>0.8596754807692307</v>
       </c>
     </row>
     <row r="72">
@@ -2369,10 +2369,10 @@
         <v>570</v>
       </c>
       <c r="C72">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D72">
-        <v>2298</v>
+        <v>2303</v>
       </c>
       <c r="E72">
         <v>3325</v>
@@ -2381,10 +2381,10 @@
         <v>0.1714285714285714</v>
       </c>
       <c r="G72">
-        <v>0.1374436090225564</v>
+        <v>0.1359398496240601</v>
       </c>
       <c r="H72">
-        <v>0.6911278195488721</v>
+        <v>0.6926315789473684</v>
       </c>
     </row>
     <row r="73">
@@ -2397,10 +2397,10 @@
         <v>299</v>
       </c>
       <c r="C73">
-        <v>846</v>
+        <v>828</v>
       </c>
       <c r="D73">
-        <v>2179</v>
+        <v>2197</v>
       </c>
       <c r="E73">
         <v>3324</v>
@@ -2409,38 +2409,94 @@
         <v>0.08995186522262334</v>
       </c>
       <c r="G73">
-        <v>0.2545126353790614</v>
+        <v>0.2490974729241877</v>
       </c>
       <c r="H73">
-        <v>0.6555354993983152</v>
+        <v>0.660950661853189</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>FSZZ130</t>
+          <t>FSZZ106</t>
         </is>
       </c>
       <c r="B74">
-        <v>1079</v>
+        <v>1395</v>
       </c>
       <c r="C74">
-        <v>857</v>
+        <v>803</v>
       </c>
       <c r="D74">
-        <v>1381</v>
+        <v>1119</v>
       </c>
       <c r="E74">
         <v>3317</v>
       </c>
       <c r="F74">
+        <v>0.4205607476635514</v>
+      </c>
+      <c r="G74">
+        <v>0.242086222490202</v>
+      </c>
+      <c r="H74">
+        <v>0.3373530298462466</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>FSZZ108</t>
+        </is>
+      </c>
+      <c r="B75">
+        <v>581</v>
+      </c>
+      <c r="C75">
+        <v>592</v>
+      </c>
+      <c r="D75">
+        <v>2149</v>
+      </c>
+      <c r="E75">
+        <v>3322</v>
+      </c>
+      <c r="F75">
+        <v>0.174894641782059</v>
+      </c>
+      <c r="G75">
+        <v>0.1782059000602047</v>
+      </c>
+      <c r="H75">
+        <v>0.6468994581577363</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>FSZZ130</t>
+        </is>
+      </c>
+      <c r="B76">
+        <v>1079</v>
+      </c>
+      <c r="C76">
+        <v>834</v>
+      </c>
+      <c r="D76">
+        <v>1404</v>
+      </c>
+      <c r="E76">
+        <v>3317</v>
+      </c>
+      <c r="F76">
         <v>0.3252939403075068</v>
       </c>
-      <c r="G74">
-        <v>0.2583659933675008</v>
-      </c>
-      <c r="H74">
-        <v>0.4163400663249925</v>
+      <c r="G76">
+        <v>0.2514320168827254</v>
+      </c>
+      <c r="H76">
+        <v>0.4232740428097679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>